<commit_message>
Modified API list csv file
</commit_message>
<xml_diff>
--- a/docs/HEYDAY-proto-backend API_list.xlsx
+++ b/docs/HEYDAY-proto-backend API_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vscode-projects\digital-transformation-server\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260C9ADA-4ED4-42C4-A892-97928CCF1E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162004C6-8B8A-4D4A-B914-A356C25E680B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="api_list" sheetId="1" r:id="rId1"/>
@@ -401,15 +401,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;center_equipment_id&gt; 장비로 하는 운동 끝내기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>req_center_equipments_auth.py</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>req_center_equipments_leave.py</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;center_equipment_id&gt; 장비 사용 마무리하기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -515,7 +515,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -544,6 +544,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -828,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1036,31 +1042,31 @@
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="3">
+      <c r="B17" s="10">
         <v>14</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="10">
+        <v>15</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="3">
-        <v>15</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="19" spans="2:5">
@@ -1313,7 +1319,7 @@
   <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1522,25 +1528,25 @@
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1553,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03F71D9-DE2C-475A-B6E7-E1A58E34F6BF}">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1895,25 +1901,25 @@
       </c>
     </row>
     <row r="32" spans="2:4">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the path of APIs
</commit_message>
<xml_diff>
--- a/docs/HEYDAY-proto-backend API_list.xlsx
+++ b/docs/HEYDAY-proto-backend API_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vscode-projects\digital-transformation-server\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162004C6-8B8A-4D4A-B914-A356C25E680B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444F18F8-31D6-4040-8D07-63EB42620CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="api_list" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="99">
   <si>
     <t>/signin</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -410,6 +410,18 @@
   </si>
   <si>
     <t>&lt;center_equipment_id&gt; 장비 사용 마무리하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/users/&lt;user_id&gt;/workouts/exercise_libraries/&lt;exercise_library_id&gt;/report/recent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/users/&lt;user_id&gt;/workouts/exercise_libraries/&lt;exercise_library_id&gt;/&lt;set_number&gt;/report/recent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>req_users_workouts_exerciselibrary_report.py</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -515,7 +527,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -550,6 +562,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -834,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1280,31 +1295,31 @@
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="3">
+      <c r="B34" s="10">
         <v>31</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D34" s="7" t="s">
+      <c r="C34" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>75</v>
+      <c r="E34" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="3">
+      <c r="B35" s="10">
         <v>32</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="C35" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>75</v>
+      <c r="E35" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1559,8 +1574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03F71D9-DE2C-475A-B6E7-E1A58E34F6BF}">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B39:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>